<commit_message>
Updated the 2-spoke spreadsheet
</commit_message>
<xml_diff>
--- a/PowerShell/ParametersFileBuilder_2-Spoke.xlsx
+++ b/PowerShell/ParametersFileBuilder_2-Spoke.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://avanade-my.sharepoint.com/personal/mark_bakunas_avanade_com/Documents/South Region/Cloud Foundations Workshop/CFW 2.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{978C28EA-4A59-47C2-B41C-9AF37265FA78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4A44D8F7-37CB-4DE5-94B9-5923CFACD555}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{6ECD824E-A4F9-44ED-BB6F-BCB980C725A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{57E61E94-3848-463A-AFFE-C79959FB6905}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="1080" windowWidth="21600" windowHeight="13650" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
+    <workbookView xWindow="2340" yWindow="495" windowWidth="21600" windowHeight="13650" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
@@ -31,46 +31,49 @@
     <definedName name="calcHubSubnetBastionAddressSpace">ParametersFile!$B$11</definedName>
     <definedName name="calcHubSubnetJumpHostsAddressSpace">ParametersFile!$B$12</definedName>
     <definedName name="dcAdminsAadGroupObjectId">General!$B$10</definedName>
+    <definedName name="dcVmContributorsRoleAssignmentID">ParametersFile!$B$19</definedName>
     <definedName name="deployOptions_List">Lists!$E$2:$E$3</definedName>
-    <definedName name="hubSubnet1AddressSpace">Hub!$C$8</definedName>
-    <definedName name="hubSubnet1Deploy">Hub!$D$8</definedName>
-    <definedName name="hubSubnet1Name">Hub!$B$8</definedName>
-    <definedName name="hubSubnet2AddressSpace">Hub!$C$9</definedName>
-    <definedName name="hubSubnet2Deploy">Hub!$D$9</definedName>
-    <definedName name="hubSubnet2Name">Hub!$B$9</definedName>
-    <definedName name="hubSubnet3AddressSpace">Hub!$C$10</definedName>
-    <definedName name="hubSubnet3Deploy">Hub!$D$10</definedName>
-    <definedName name="hubSubnet3Name">Hub!$B$10</definedName>
-    <definedName name="hubSubnet4AddressSpace">Hub!$C$11</definedName>
-    <definedName name="hubSubnet4Deploy">Hub!$D$11</definedName>
-    <definedName name="hubSubnet4Name">Hub!$B$11</definedName>
-    <definedName name="hubSubnetBastionAddressSpace">Hub!$C$5</definedName>
-    <definedName name="hubSubnetBastionDeploy">Hub!$D$5</definedName>
-    <definedName name="hubSubnetDcAddressSpace">Hub!$C$6</definedName>
-    <definedName name="hubSubnetDcName">Hub!$B$6</definedName>
-    <definedName name="hubSubnetFirewallAddressSpace">Hub!$C$4</definedName>
-    <definedName name="hubSubnetFirewallDeploy">Hub!$D$4</definedName>
-    <definedName name="hubSubnetGatewayAddressSpace">Hub!$C$3</definedName>
-    <definedName name="hubSubnetJumpHostsAddressSpace">Hub!$C$7</definedName>
-    <definedName name="hubSubnetJumpHostsDeploy">Hub!$D$7</definedName>
-    <definedName name="hubSubnetJumpHostsName">Hub!$B$7</definedName>
+    <definedName name="hubSubnet1AddressSpace">Hub!$C$9</definedName>
+    <definedName name="hubSubnet1Deploy">Hub!$D$9</definedName>
+    <definedName name="hubSubnet1Name">Hub!$B$9</definedName>
+    <definedName name="hubSubnet2AddressSpace">Hub!$C$10</definedName>
+    <definedName name="hubSubnet2Deploy">Hub!$D$10</definedName>
+    <definedName name="hubSubnet2Name">Hub!$B$10</definedName>
+    <definedName name="hubSubnet3AddressSpace">Hub!$C$11</definedName>
+    <definedName name="hubSubnet3Deploy">Hub!$D$11</definedName>
+    <definedName name="hubSubnet3Name">Hub!$B$11</definedName>
+    <definedName name="hubSubnet4AddressSpace">Hub!$C$12</definedName>
+    <definedName name="hubSubnet4Deploy">Hub!$D$12</definedName>
+    <definedName name="hubSubnet4Name">Hub!$B$12</definedName>
+    <definedName name="hubSubnetBastionAddressSpace">Hub!$C$6</definedName>
+    <definedName name="hubSubnetBastionDeploy">Hub!$D$6</definedName>
+    <definedName name="hubSubnetDcAddressSpace">Hub!$C$7</definedName>
+    <definedName name="hubSubnetDcName">Hub!$B$7</definedName>
+    <definedName name="hubSubnetFirewallAddressSpace">Hub!$C$5</definedName>
+    <definedName name="hubSubnetFirewallDeploy">Hub!$D$5</definedName>
+    <definedName name="hubSubnetGatewayAddressSpace">Hub!$C$4</definedName>
+    <definedName name="hubSubnetJumpHostsAddressSpace">Hub!$C$8</definedName>
+    <definedName name="hubSubnetJumpHostsDeploy">Hub!$D$8</definedName>
+    <definedName name="hubSubnetJumpHostsName">Hub!$B$8</definedName>
+    <definedName name="hubSubnetVmContRoleAssignmantId">ParametersFile!$B$20</definedName>
     <definedName name="hubVnetAddressSpace">Hub!$C$2</definedName>
     <definedName name="hubVnetName">Hub!$B$2</definedName>
     <definedName name="routeTableName">General!$B$7</definedName>
     <definedName name="serverTeamAadGroupObjectId">General!$B$11</definedName>
-    <definedName name="spokeDeploySubscriptionResourceGroup">ParametersFile!$B$22</definedName>
-    <definedName name="spokeSubnet1AddressSpace">ParametersFile!$B$27</definedName>
-    <definedName name="spokeSubnet1Name">ParametersFile!$B$26</definedName>
-    <definedName name="spokeSubnet2AddressSpace">ParametersFile!$B$29</definedName>
-    <definedName name="spokeSubnet2Name">ParametersFile!$B$28</definedName>
-    <definedName name="spokeSubnet3AddressSpace">ParametersFile!$B$31</definedName>
-    <definedName name="spokeSubnet3Name">ParametersFile!$B$30</definedName>
-    <definedName name="spokeSubnetAppGwAddressSpace">ParametersFile!$B$25</definedName>
-    <definedName name="spokeSubnetAppGwName">ParametersFile!$B$24</definedName>
-    <definedName name="spokeSubnetBastionAddressSpace">ParametersFile!$B$23</definedName>
+    <definedName name="spokeDeploySubscriptionResourceGroup">ParametersFile!$B$26</definedName>
+    <definedName name="spokeSubnet1AddressSpace">ParametersFile!$B$31</definedName>
+    <definedName name="spokeSubnet1Name">ParametersFile!$B$30</definedName>
+    <definedName name="spokeSubnet2AddressSpace">ParametersFile!$B$33</definedName>
+    <definedName name="spokeSubnet2Name">ParametersFile!$B$32</definedName>
+    <definedName name="spokeSubnet3AddressSpace">ParametersFile!$B$35</definedName>
+    <definedName name="spokeSubnet3Name">ParametersFile!$B$34</definedName>
+    <definedName name="spokeSubnetAppGwAddressSpace">ParametersFile!$B$29</definedName>
+    <definedName name="spokeSubnetAppGwName">ParametersFile!$B$28</definedName>
+    <definedName name="spokeSubnetBastionAddressSpace">ParametersFile!$B$27</definedName>
     <definedName name="spokeSubnetUniqueness_List">Lists!$G$2:$G$3</definedName>
-    <definedName name="spokeVnetAddressSpace">ParametersFile!$B$21</definedName>
-    <definedName name="spokeVnetName">ParametersFile!$B$20</definedName>
+    <definedName name="spokeVmContributorsRoleAssignmentID">ParametersFile!$B$36</definedName>
+    <definedName name="spokeVnetAddressSpace">ParametersFile!$B$25</definedName>
+    <definedName name="spokeVnetName">ParametersFile!$B$24</definedName>
     <definedName name="vnetDdosProtectionLevel">General!$B$4</definedName>
     <definedName name="vnetDdosProtectionLevel_List">Lists!$A$2:$A$4</definedName>
     <definedName name="vnetDdosProtectionPlanName">General!$B$5</definedName>
@@ -95,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="131">
   <si>
     <t>Name</t>
   </si>
@@ -232,12 +235,6 @@
     <t>RBAC</t>
   </si>
   <si>
-    <t>Server Team</t>
-  </si>
-  <si>
-    <t>App Teams</t>
-  </si>
-  <si>
     <t>Role</t>
   </si>
   <si>
@@ -262,9 +259,6 @@
     <t>17ba8236-a5e8-4173-8ce9-c69b17743ac2</t>
   </si>
   <si>
-    <t>DC Admins</t>
-  </si>
-  <si>
     <t>184540aa-dae3-42cd-a5aa-0f1c34c17d98</t>
   </si>
   <si>
@@ -421,9 +415,6 @@
     <t>High</t>
   </si>
   <si>
-    <t>Azure AD goup object ID</t>
-  </si>
-  <si>
     <t>Deploy</t>
   </si>
   <si>
@@ -464,6 +455,42 @@
   </si>
   <si>
     <t>Common</t>
+  </si>
+  <si>
+    <t>spokeVmContributorsRoleAssignmentID</t>
+  </si>
+  <si>
+    <t>Azure AD group object ID</t>
+  </si>
+  <si>
+    <t>Sopke VM contributors</t>
+  </si>
+  <si>
+    <t>Spoke VM contrib.</t>
+  </si>
+  <si>
+    <t>HubDCs subnet VM contributors</t>
+  </si>
+  <si>
+    <t>Hub other subnets VM contributors</t>
+  </si>
+  <si>
+    <t>DCs subnet VM contrib</t>
+  </si>
+  <si>
+    <t>other subnets VM contrib</t>
+  </si>
+  <si>
+    <t>Required</t>
+  </si>
+  <si>
+    <t>hubSubnetVmContRoleAssignmantId</t>
+  </si>
+  <si>
+    <t>dcVmContributorsRoleAssignmentID</t>
+  </si>
+  <si>
+    <t>Hub Array Values</t>
   </si>
 </sst>
 </file>
@@ -526,14 +553,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
@@ -864,17 +894,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -882,7 +912,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -890,7 +920,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -898,47 +928,47 @@
         <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>123</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>124</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>121</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -960,7 +990,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC352499-16C6-4142-B6A7-FED4572A9C0C}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -974,7 +1004,7 @@
     <col min="4" max="5" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -982,7 +1012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -993,247 +1023,287 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="D6" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="D8" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="D9" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="D10" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D10" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="D11" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="D12" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>44</v>
       </c>
-      <c r="B13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" t="str">
+        <f>IF(dcAdminsAadGroupObjectId = "", "Not needed", "Required")</f>
+        <v>Required</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>55</v>
-      </c>
-      <c r="B14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="E17" t="str">
+        <f>IF(hubSubnetJumpHostsDeploy = "Deploy", "Required", "Not Needed")</f>
+        <v>Required</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="E18" s="7" t="str">
+        <f>IF(hubSubnet1Deploy = "Don't Deploy", "Not Needed", "Required")</f>
+        <v>Required</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E19" s="7" t="str">
+        <f>IF(
+OR(hubSubnet1Deploy = "Don't Deploy", hubSubnet2Deploy = "Don't Deploy"),
+"Not Needed", "Required")</f>
+        <v>Required</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="7" t="str">
+        <f>IF(
+OR(hubSubnet1Deploy = "Don't Deploy", hubSubnet2Deploy = "Don't Deploy", hubSubnet3Deploy = "Don't Deploy"),
+"Not Needed", "Required")</f>
+        <v>Required</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" s="7" t="str">
+        <f>IF(
+OR(hubSubnet1Deploy = "Don't Deploy", hubSubnet2Deploy = "Don't Deploy", hubSubnet3Deploy = "Don't Deploy", hubSubnet4Deploy = "Don't Deploy"),
+"Not Needed", "Required")</f>
+        <v>Required</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>103</v>
+      <c r="D22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D4:D5 D7:D11" xr:uid="{D9354EF7-27D1-4C1F-B57B-07A789DEC96E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D6 D8:D12" xr:uid="{D9354EF7-27D1-4C1F-B57B-07A789DEC96E}">
       <formula1>deployOptions_List</formula1>
     </dataValidation>
   </dataValidations>
@@ -1244,7 +1314,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D3422A-C2D2-42AC-9F3F-3909382DD971}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -1266,7 +1336,7 @@
         <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1299,133 +1369,128 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>122</v>
-      </c>
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
+      <c r="D11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
         <v>45</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
         <v>48</v>
-      </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" t="s">
         <v>46</v>
-      </c>
-      <c r="B14" t="s">
-        <v>48</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D7 D9:D10" xr:uid="{0CD32938-FC7D-4A2D-89DA-FA2CAD0BA150}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D8 D10:D11" xr:uid="{0CD32938-FC7D-4A2D-89DA-FA2CAD0BA150}">
       <formula1>deployOptions_List</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E10" xr:uid="{EBB888DC-D06B-428F-9A6F-3A30046B1109}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E7:E11" xr:uid="{EBB888DC-D06B-428F-9A6F-3A30046B1109}">
       <formula1>spokeSubnetUniqueness_List</formula1>
     </dataValidation>
   </dataValidations>
@@ -1436,7 +1501,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A2061D0-44C8-4698-9DEF-5B9D4440337D}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -1458,7 +1523,7 @@
         <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1466,10 +1531,10 @@
         <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D2" t="str">
         <f>IF(B2 &lt;&gt; "", _xlfn.CONCAT(CHAR(34), B2, "/", C2, CHAR(34)), _xlfn.CONCAT("""", """"))</f>
@@ -1489,39 +1554,25 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" t="str">
-        <f>Spoke1!E6</f>
-        <v>Common</v>
-      </c>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E7" t="str">
         <f>Spoke1!E7</f>
@@ -1530,13 +1581,16 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="E8" t="str">
         <f>Spoke1!E8</f>
@@ -1545,16 +1599,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="E9" t="str">
         <f>Spoke1!E9</f>
@@ -1563,67 +1614,76 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E10" t="str">
         <f>Spoke1!E10</f>
         <v>Common</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" t="str">
+        <f>Spoke1!E11</f>
+        <v>Common</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
         <v>45</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
         <v>48</v>
       </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" t="s">
         <v>46</v>
-      </c>
-      <c r="B14" t="s">
-        <v>48</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D7 D9:D10" xr:uid="{01786FD6-A133-4CF7-BD55-62BA227952C7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:D8 D10:D11" xr:uid="{01786FD6-A133-4CF7-BD55-62BA227952C7}">
       <formula1>deployOptions_List</formula1>
     </dataValidation>
   </dataValidations>
@@ -1634,7 +1694,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E5F0421-4CC3-4847-AE8E-9E8CD1C6E8C6}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -1648,16 +1708,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="3" t="str">
+        <v>73</v>
+      </c>
+      <c r="B1" s="4" t="str">
         <f>_xlfn.CONCAT(B3, ",", B4, ",", B5,  B6)</f>
-        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"vnetDdosProtectionLevel": {"value":"Basic"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-01"},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"10.0.0.128/26"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcVmContributorsAadGroupId": {"value":"17ba8236-a5e8-4173-8ce9-c69b17743ac2"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0","0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24"]}}}</v>
+        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"vnetDdosProtectionLevel": {"value":"Standard - Create New"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-01"},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"17ba8236-a5e8-4173-8ce9-c69b17743ac2"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"5eb970ea-e71a-4bf9-ba78-0529b3aeb2f3"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24"]},"spokeVmContAadGroupId": {"value":["c2ecad99-6ed7-4e11-8acc-0fa0262a2c69"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6"]}}}</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B3" t="str">
         <f>_xlfn.CONCAT("{",
@@ -1670,12 +1730,12 @@
 CHAR(34),"vnetNsgSecurityLevel",CHAR(34),": {",CHAR(34),"value",CHAR(34),":",CHAR(34),vnetNsgSecurityLevel,CHAR(34),"},",
 CHAR(34),"routeTableName",CHAR(34),": {",CHAR(34),"value",CHAR(34),":",CHAR(34),routeTableName,CHAR(34),"}"
 )</f>
-        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"vnetDdosProtectionLevel": {"value":"Basic"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-01"}</v>
+        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"vnetDdosProtectionLevel": {"value":"Standard - Create New"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-01"}</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B4" t="str">
         <f>_xlfn.CONCAT(
@@ -1696,15 +1756,17 @@
 CHAR(34), "hubSubnet3AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), calcHubSubnet3AddressSpace, CHAR(34), "},",
 CHAR(34), "hubSubnet4Name", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), hubSubnet4Name, CHAR(34), "},",
 CHAR(34), "hubSubnet4AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), calcHubSubnet4AddressSpace, CHAR(34), "},",
-CHAR(34), "dcVmContributorsAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), dcAdminsAadGroupObjectId, CHAR(34), "},",
-CHAR(34), "dcVmContributorsRoleAssignmentID", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", CHAR(34), Hub!D14, CHAR(34), ",", CHAR(34),Hub!D15, CHAR(34), "]}",
+CHAR(34), "dcSubnetVmContAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), dcAdminsAadGroupObjectId, CHAR(34), "},",
+CHAR(34), "dcVmContributorsRoleAssignmentID", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", dcVmContributorsRoleAssignmentID, "]},",
+CHAR(34), "hubSubnetVmContAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), serverTeamAadGroupObjectId, CHAR(34), "},",
+CHAR(34), "hubSubnetVmContRoleAssignmantId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", hubSubnetVmContRoleAssignmantId, "]}"
 )</f>
-        <v>"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"10.0.0.128/26"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcVmContributorsAadGroupId": {"value":"17ba8236-a5e8-4173-8ce9-c69b17743ac2"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]}</v>
+        <v>"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"17ba8236-a5e8-4173-8ce9-c69b17743ac2"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"5eb970ea-e71a-4bf9-ba78-0529b3aeb2f3"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]}</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B5" t="str">
         <f>_xlfn.CONCAT(
@@ -1719,14 +1781,16 @@
 CHAR(34), "spokeSubnet2Name", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeSubnet2Name,"]},",
 CHAR(34), "spokeSubnet2AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeSubnet2AddressSpace,"]},",
 CHAR(34), "spokeSubnet3Name", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeSubnet3Name,"]},",
-CHAR(34), "spokeSubnet3AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeSubnet3AddressSpace,"]}"
+CHAR(34), "spokeSubnet3AddressSpace", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeSubnet3AddressSpace,"]},",
+CHAR(34), "spokeVmContAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", CHAR(34), appTeamsAadGroupObjectId, CHAR(34), "]},",
+CHAR(34), "spokeVmContributorsRoleAssignmentID", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeVmContributorsRoleAssignmentID,"]}"
 )</f>
-        <v>"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0","0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24"]}</v>
+        <v>"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24"]},"spokeVmContAadGroupId": {"value":["c2ecad99-6ed7-4e11-8acc-0fa0262a2c69"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6"]}</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B6" t="str">
         <f>_xlfn.CONCAT(
@@ -1736,14 +1800,14 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B9" s="5"/>
+      <c r="A9" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="8"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B10" t="str">
         <f>IF(hubSubnetFirewallDeploy = "Deploy", hubSubnetFirewallAddressSpace, "0.0.0.0/0")</f>
@@ -1752,16 +1816,16 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B11" t="str">
         <f>IF(hubSubnetBastionDeploy = "Deploy", hubSubnetBastionAddressSpace, "0.0.0.0/0")</f>
-        <v>10.0.0.128/26</v>
+        <v>0.0.0.0/0</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B12" t="str">
         <f>IF(hubSubnetJumpHostsDeploy = "Deploy", hubSubnetJumpHostsAddressSpace, "0.0.0.0/0")</f>
@@ -1770,7 +1834,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B13" t="str">
         <f>IF(hubSubnet1Deploy = "Deploy", hubSubnet1AddressSpace, "0.0.0.0/0")</f>
@@ -1779,7 +1843,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B14" t="str">
         <f>IF(
@@ -1791,7 +1855,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B15" t="str">
         <f>IF(
@@ -1803,7 +1867,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B16" t="str">
         <f>IF(
@@ -1813,174 +1877,234 @@
         <v>10.0.1.96/27</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" s="5"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B20" t="str">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B19" s="7" t="str">
+        <f>_xlfn.CONCAT("""", Hub!D15, """", ",", """", Hub!D16, """")</f>
+        <v>"184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="7" t="str">
+        <f>_xlfn.CONCAT(
+"""", Hub!D22, """",
+IF(Hub!E17 = "Required", "," &amp; """" &amp; Hub!D17 &amp; """", ""),
+IF(Hub!E18 = "Required", "," &amp; """" &amp; Hub!D18 &amp; """", ""),
+IF(Hub!E19 = "Required", "," &amp; """" &amp; Hub!D19 &amp; """", ""),
+IF(Hub!E20 = "Required", "," &amp; """" &amp; Hub!D20 &amp; """", ""),
+IF(Hub!E21 = "Required", "," &amp; """" &amp; Hub!D21 &amp; """", "")
+)</f>
+        <v>"0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="8"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" t="str">
         <f>_xlfn.CONCAT(CHAR(34), Spoke1!$B$5, CHAR(34), ",", CHAR(34), Spoke2!$B$5, CHAR(34))</f>
         <v>"Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01"</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>88</v>
-      </c>
-      <c r="B21" t="str">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" t="str">
         <f>_xlfn.CONCAT(CHAR(34), Spoke1!$C$5, CHAR(34), ",", CHAR(34), Spoke2!$C$5, CHAR(34))</f>
         <v>"10.1.0.0/16","10.2.0.0/16"</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>89</v>
-      </c>
-      <c r="B22" t="str">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" t="str">
         <f>_xlfn.CONCAT(Spoke1!$D$2, ",", Spoke2!$D$2)</f>
         <v>"","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02"</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" t="str">
-        <f>_xlfn.CONCAT(
-IF(Spoke1!$D$6 = "Don't Deploy", """" &amp; "0.0.0.0/0" &amp; """" &amp; ",", """" &amp; Spoke1!$C$6 &amp; """" &amp; ","),
-IF(
-OR(AND(Spoke1!$E$6 = "Common", Spoke1!$D$6 = "Don't Deploy"), AND(Spoke1!$E$6 = "Unique", Spoke2!$D$6 = "Don't Deploy")),
-"""" &amp; "0.0.0.0/0" &amp; """",
-"""" &amp; Spoke2!$C$6 &amp; """"
-))</f>
-        <v>"0.0.0.0/0","0.0.0.0/0"</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>92</v>
-      </c>
-      <c r="B24" s="4" t="str">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B27" t="str">
         <f>IF(
 Spoke1!$E$7 = "Common",
-"""" &amp; Spoke1!$B$7 &amp; """",
-_xlfn.CONCAT("""", Spoke1!$B$7, """", ",", """", Spoke2!$B$7, """")
+IF(Spoke1!$D$7 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$7 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$7  &amp; """"),
+_xlfn.CONCAT(
+"""",
+IF(Spoke1!$D$7 = "Don't Deploy", "0.0.0.0/0", Spoke1!$C$7),
+"""", ",", """",
+IF(Spoke2!$D$7 = "Don't Deploy", "0.0.0.0/0", Spoke2!$C$7),
+""""
+)
+)</f>
+        <v>"0.0.0.0/0"</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B28" s="5" t="str">
+        <f>IF(
+Spoke1!$E$8 = "Common",
+"""" &amp; Spoke1!$B$8 &amp; """",
+_xlfn.CONCAT("""", Spoke1!$B$8, """", ",", """", Spoke2!$B$8, """")
 )</f>
         <v>"AppGW"</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>93</v>
-      </c>
-      <c r="B25" t="str">
-        <f>_xlfn.CONCAT(
-IF(Spoke1!$D$7 = "Don't Deploy", """" &amp; "0.0.0.0/0" &amp; """" &amp; ",", """" &amp; Spoke1!$C$7 &amp; """" &amp; ","),
-IF(
-OR(AND(Spoke1!$E$7 = "Common", Spoke1!$D$7 = "Don't Deploy"), AND(Spoke1!$E$7 = "Unique", Spoke2!$D$7 = "Don't Deploy")),
-"""" &amp; "0.0.0.0/0" &amp; """",
-"""" &amp; Spoke2!$C$7 &amp; """"
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="3" t="str">
+        <f>IF(
+Spoke1!$E$8 = "Common",
+IF(Spoke1!$D$8 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$8 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$8  &amp; """"),
+_xlfn.CONCAT(
+"""",
+IF(Spoke1!$D$8 = "Don't Deploy", "0.0.0.0/0", Spoke1!$C$8),
+"""", ",", """",
+IF(Spoke2!$D$8 = "Don't Deploy", "0.0.0.0/0", Spoke2!$C$8),
+""""
 )
 )</f>
         <v>"10.1.0.128/25","10.2.0.128/25"</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" s="4" t="str">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="5" t="str">
         <f>IF(
-Spoke1!$E$7 = "Common",
-"""" &amp; Spoke1!$B$8 &amp; """",
-_xlfn.CONCAT("""", Spoke1!$B$8, """", ",", """", Spoke2!$B$8, """")
+Spoke1!$E$8 = "Common",
+"""" &amp; Spoke1!$B$9 &amp; """",
+_xlfn.CONCAT("""", Spoke1!$B$9, """", ",", """", Spoke2!$B$9, """")
 )</f>
         <v>"Subnet1"</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" t="str">
-        <f>_xlfn.CONCAT(
-IF(Spoke1!$D$8 = "Don't Deploy", """" &amp; "0.0.0.0/0" &amp; """" &amp; ",", """" &amp; Spoke1!$C$8 &amp; """" &amp; ","),
-IF(
-OR(AND(Spoke1!$E$8 = "Common", Spoke1!$D$8 = "Don't Deploy"), AND(Spoke1!$E$8 = "Unique", Spoke2!$D$8 = "Don't Deploy")),
-"""" &amp; "0.0.0.0/0" &amp; """",
- """" &amp; Spoke2!$C$8 &amp; """"
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31" s="3" t="str">
+        <f>IF(
+Spoke1!$E$9 = "Common",
+IF(Spoke1!$D$9 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$9 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$9  &amp; """"),
+_xlfn.CONCAT(
+"""",
+IF(Spoke1!$D$9 = "Don't Deploy", "0.0.0.0/0", Spoke1!$C$9),
+"""", ",", """",
+IF(Spoke2!$D$9 = "Don't Deploy", "0.0.0.0/0", Spoke2!$C$9),
+""""
 )
 )</f>
         <v>"10.1.1.0/24","10.2.1.0/24"</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>98</v>
-      </c>
-      <c r="B28" s="4" t="str">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32" s="5" t="str">
         <f>IF(
-Spoke1!$E$9 = "Common",
-"""" &amp; Spoke1!$B$9 &amp; """",
-_xlfn.CONCAT("""", Spoke1!$B$9, """", ",", """", Spoke2!$B$9, """")
+Spoke1!$E$10 = "Common",
+"""" &amp; Spoke1!$B$10 &amp; """",
+_xlfn.CONCAT("""", Spoke1!$B$10, """", ",", """", Spoke2!$B$10, """")
 )</f>
         <v>"Subnet2"</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>99</v>
-      </c>
-      <c r="B29" t="str">
-        <f>_xlfn.CONCAT(
-IF(Spoke1!$D$9 = "Don't Deploy", """" &amp; "0.0.0.0/0" &amp; """" &amp; ",", """" &amp; Spoke1!$C$9 &amp; """" &amp; ","),
-IF(
-OR(AND(Spoke1!$E$9 = "Common", Spoke1!$D$9 = "Don't Deploy"), AND(Spoke1!$E$9 = "Unique", Spoke2!$D$9 = "Don't Deploy")),
-"""" &amp; "0.0.0.0/0" &amp; """",
- """" &amp; Spoke2!$C$9 &amp; """"
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="3" t="str">
+        <f>IF(
+Spoke1!$E$10 = "Common",
+IF(Spoke1!$D$10 = "Don't Deploy", """"  &amp; "0.0.0.0/0" &amp; """", """" &amp;  Spoke1!$C$10 &amp; """" &amp; "," &amp;   """" &amp; Spoke2!$C$10  &amp; """"),
+_xlfn.CONCAT(
+"""",
+IF(Spoke1!$D$10 = "Don't Deploy", "0.0.0.0/0", Spoke1!$C$10),
+"""", ",", """",
+IF(Spoke2!$D$10 = "Don't Deploy", "0.0.0.0/0", Spoke2!$C$10),
+""""
 )
 )</f>
         <v>"10.1.2.0/24","10.2.2.0/24"</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>100</v>
-      </c>
-      <c r="B30" s="4" t="str">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>97</v>
+      </c>
+      <c r="B34" s="5" t="str">
         <f>IF(
-Spoke1!$E$7 = "Common",
-"""" &amp; Spoke1!$B$10 &amp; """",
-_xlfn.CONCAT("""", Spoke1!$B$10, """", ",", """", Spoke2!$B$10, """")
+Spoke1!$E$8 = "Common",
+"""" &amp; Spoke1!$B$11 &amp; """",
+_xlfn.CONCAT("""", Spoke1!$B$11, """", ",", """", Spoke2!$B$11, """")
 )</f>
         <v>"Subnet3"</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>101</v>
-      </c>
-      <c r="B31" t="str">
-        <f>_xlfn.CONCAT(
-IF(Spoke1!$D$10 = "Don't Deploy", """" &amp; "0.0.0.0/0" &amp; """" &amp; ",", """" &amp; Spoke1!$C$10 &amp; """" &amp; ","),
-IF(
-OR(AND(Spoke1!$E$10 = "Common", Spoke1!$D$10 = "Don't Deploy"), AND(Spoke1!$E$10 = "Unique", Spoke2!$D$10 = "Don't Deploy")),
-"""" &amp; "0.0.0.0/0" &amp; """",
- """" &amp; Spoke2!$C$10 &amp; """"
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>98</v>
+      </c>
+      <c r="B35" s="3" t="str">
+        <f>IF(
+Spoke1!$E$11 = "Common",
+IF(OR(Spoke1!$D$11 = "Don't Deploy", Spoke1!$D$10 = "Don't Deploy"),
+ """"  &amp; "0.0.0.0/0" &amp; """",
+ """" &amp;  IF(Spoke1!$D$10 = "Don't Deploy", "0.0.0.0/0", Spoke1!$C$11) &amp; """" &amp; "," &amp;
+"""" &amp; IF(Spoke2!$D$10 = "Don't Deploy", "0.0.0.0/0", Spoke2!$C$11) ) &amp; """",
+_xlfn.CONCAT(
+"""",
+IF(OR(Spoke1!$D$11 = "Don't Deploy", Spoke1!$D$10 = "Don't Deploy"), "0.0.0.0/0", Spoke1!$C$11),
+"""", ",", """",
+IF(OR(Spoke2!$D$11 = "Don't Deploy", Spoke2!$D$10 = "Don't Deploy"), "0.0.0.0/0", Spoke2!$C$11),
+""""
 )
 )</f>
         <v>"10.1.3.0/24","10.2.3.0/24"</v>
       </c>
     </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>119</v>
+      </c>
+      <c r="B36" t="str">
+        <f>_xlfn.CONCAT("""",Spoke1!D15,"""",",","""",Spoke2!D15,"""")</f>
+        <v>"5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6"</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A23:B23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2011,46 +2135,46 @@
         <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated group OIDs for new tenant
</commit_message>
<xml_diff>
--- a/PowerShell/ParametersFileBuilder_2-Spoke.xlsx
+++ b/PowerShell/ParametersFileBuilder_2-Spoke.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://avanade-my.sharepoint.com/personal/mark_bakunas_avanade_com/Documents/South Region/Cloud Foundations Workshop/CFW 2.0/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark.bakunas\Documents\GitHub\Azure-HubSpoke\PowerShell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{6ECD824E-A4F9-44ED-BB6F-BCB980C725A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{57E61E94-3848-463A-AFFE-C79959FB6905}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E31DB652-6946-4AEB-B6A6-2596311D069B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="495" windowWidth="21600" windowHeight="13650" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
+    <workbookView xWindow="4710" yWindow="945" windowWidth="21600" windowHeight="13650" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
@@ -241,9 +241,6 @@
     <t>VM contributor</t>
   </si>
   <si>
-    <t>5eb970ea-e71a-4bf9-ba78-0529b3aeb2f3</t>
-  </si>
-  <si>
     <t>Role assignment GUID</t>
   </si>
   <si>
@@ -253,12 +250,6 @@
     <t>5a29e932-06c6-4e07-8e1b-d5f96c3524cf</t>
   </si>
   <si>
-    <t>c2ecad99-6ed7-4e11-8acc-0fa0262a2c69</t>
-  </si>
-  <si>
-    <t>17ba8236-a5e8-4173-8ce9-c69b17743ac2</t>
-  </si>
-  <si>
     <t>184540aa-dae3-42cd-a5aa-0f1c34c17d98</t>
   </si>
   <si>
@@ -491,6 +482,15 @@
   </si>
   <si>
     <t>Hub Array Values</t>
+  </si>
+  <si>
+    <t>83578c91-9919-4bd8-bee8-2649f6eb7c13</t>
+  </si>
+  <si>
+    <t>57f2ff92-300b-4075-a7ab-2030b46ebe2f</t>
+  </si>
+  <si>
+    <t>002984bd-b5ce-445d-8138-d19b514550c7</t>
   </si>
 </sst>
 </file>
@@ -889,7 +889,7 @@
   <dimension ref="A2:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B10" sqref="B10:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,10 +901,10 @@
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -912,7 +912,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -920,7 +920,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -928,47 +928,47 @@
         <v>31</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>52</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>47</v>
+        <v>129</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>51</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -1043,7 +1043,7 @@
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1054,7 +1054,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1079,7 +1079,7 @@
         <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1093,7 +1093,7 @@
         <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1107,7 +1107,7 @@
         <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1121,7 +1121,7 @@
         <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1135,7 +1135,7 @@
         <v>28</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1146,41 +1146,41 @@
         <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B15" t="s">
         <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E16" t="str">
         <f>IF(dcAdminsAadGroupObjectId = "", "Not needed", "Required")</f>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B17" t="s">
         <v>46</v>
@@ -1198,7 +1198,7 @@
         <v>6</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E17" t="str">
         <f>IF(hubSubnetJumpHostsDeploy = "Deploy", "Required", "Not Needed")</f>
@@ -1207,7 +1207,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B18" t="s">
         <v>46</v>
@@ -1216,7 +1216,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E18" s="7" t="str">
         <f>IF(hubSubnet1Deploy = "Don't Deploy", "Not Needed", "Required")</f>
@@ -1225,7 +1225,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B19" t="s">
         <v>46</v>
@@ -1234,7 +1234,7 @@
         <v>9</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E19" s="7" t="str">
         <f>IF(
@@ -1245,7 +1245,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B20" t="s">
         <v>46</v>
@@ -1254,7 +1254,7 @@
         <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E20" s="7" t="str">
         <f>IF(
@@ -1265,7 +1265,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B21" t="s">
         <v>46</v>
@@ -1274,7 +1274,7 @@
         <v>11</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E21" s="7" t="str">
         <f>IF(
@@ -1285,19 +1285,19 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E22" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1336,7 +1336,7 @@
         <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1381,10 +1381,10 @@
         <v>37</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1398,10 +1398,10 @@
         <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1415,7 +1415,7 @@
         <v>38</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1429,10 +1429,10 @@
         <v>39</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1446,10 +1446,10 @@
         <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1460,15 +1460,15 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B14" t="s">
         <v>46</v>
@@ -1477,12 +1477,12 @@
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1523,7 +1523,7 @@
         <v>43</v>
       </c>
       <c r="D1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1531,10 +1531,10 @@
         <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D2" t="str">
         <f>IF(B2 &lt;&gt; "", _xlfn.CONCAT(CHAR(34), B2, "/", C2, CHAR(34)), _xlfn.CONCAT("""", """"))</f>
@@ -1554,10 +1554,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1569,10 +1569,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E7" t="str">
         <f>Spoke1!E7</f>
@@ -1587,10 +1587,10 @@
         <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E8" t="str">
         <f>Spoke1!E8</f>
@@ -1605,7 +1605,7 @@
         <v>21</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E9" t="str">
         <f>Spoke1!E9</f>
@@ -1620,10 +1620,10 @@
         <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E10" t="str">
         <f>Spoke1!E10</f>
@@ -1638,10 +1638,10 @@
         <v>23</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E11" t="str">
         <f>Spoke1!E11</f>
@@ -1656,15 +1656,15 @@
         <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B14" t="s">
         <v>46</v>
@@ -1673,12 +1673,12 @@
         <v>2</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D15" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1708,16 +1708,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B1" s="4" t="str">
         <f>_xlfn.CONCAT(B3, ",", B4, ",", B5,  B6)</f>
-        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"vnetDdosProtectionLevel": {"value":"Standard - Create New"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-01"},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"17ba8236-a5e8-4173-8ce9-c69b17743ac2"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"5eb970ea-e71a-4bf9-ba78-0529b3aeb2f3"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24"]},"spokeVmContAadGroupId": {"value":["c2ecad99-6ed7-4e11-8acc-0fa0262a2c69"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6"]}}}</v>
+        <v>{"$schema":"https://schema.management.azure.com/schemas/2019-04-01/deploymentParameters.json#","contentVersion":"1.0.0.0","parameters":{"assetLocationURI": {"value":"https://raw.githubusercontent.com/mbakunas/Azure-HubSpoke/master/"},"vnetDdosProtectionLevel": {"value":"Standard - Create New"},"vnetDdosProtectionPlanName": {"value":"DDOS-Plan-01"},"vnetNsgSecurityLevel": {"value":"Medium"},"routeTableName": {"value":"RouteTable-01"},"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"83578c91-9919-4bd8-bee8-2649f6eb7c13"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"57f2ff92-300b-4075-a7ab-2030b46ebe2f"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]},"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24"]},"spokeVmContAadGroupId": {"value":["002984bd-b5ce-445d-8138-d19b514550c7"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6"]}}}</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B3" t="str">
         <f>_xlfn.CONCAT("{",
@@ -1735,7 +1735,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B4" t="str">
         <f>_xlfn.CONCAT(
@@ -1761,12 +1761,12 @@
 CHAR(34), "hubSubnetVmContAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":",CHAR(34), serverTeamAadGroupObjectId, CHAR(34), "},",
 CHAR(34), "hubSubnetVmContRoleAssignmantId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", hubSubnetVmContRoleAssignmantId, "]}"
 )</f>
-        <v>"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"17ba8236-a5e8-4173-8ce9-c69b17743ac2"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"5eb970ea-e71a-4bf9-ba78-0529b3aeb2f3"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]}</v>
+        <v>"hubVnetName": {"value":"HUB-EastUS2-01"},"hubVnetAddressSpace": {"value":"10.0.0.0/23"},"hubSubnetGatewayAddressSpace": {"value":"10.0.0.0/26"},"hubSubnetFirewallAddressSpace": {"value":"10.0.0.64/26"},"hubSubnetBastionAddressSpace": {"value":"0.0.0.0/0"},"hubSubnetDcName": {"value":"Infra"},"hubSubnetDcAddressSpace": {"value":"10.0.0.192/27"},"hubSubnetJumpHostsName": {"value":"JumpHosts"},"hubSubnetJumpHostsAddressSpace": {"value":"10.0.0.224/27"},"hubSubnet1Name": {"value":"Subnet1"},"hubSubnet1AddressSpace": {"value":"10.0.1.0/27"},"hubSubnet2Name": {"value":"Subnet2"},"hubSubnet2AddressSpace": {"value":"10.0.1.32/27"},"hubSubnet3Name": {"value":"Subnet3"},"hubSubnet3AddressSpace": {"value":"10.0.1.64/27"},"hubSubnet4Name": {"value":"Subnet4"},"hubSubnet4AddressSpace": {"value":"10.0.1.96/27"},"dcSubnetVmContAadGroupId": {"value":"83578c91-9919-4bd8-bee8-2649f6eb7c13"},"dcVmContributorsRoleAssignmentID": {"value":["184540aa-dae3-42cd-a5aa-0f1c34c17d98","bde41287-27a2-4a80-b587-6ac6d56a303a"]},"hubSubnetVmContAadGroupId": {"value":"57f2ff92-300b-4075-a7ab-2030b46ebe2f"},"hubSubnetVmContRoleAssignmantId": {"value":["0702dcd4-0b65-4ebb-8ebd-873e2729904b","594fd8bf-f554-4272-8b19-9725c7b706b4","b3f5340d-28be-4029-bc10-56af7e20ac75","7a1689a7-66d8-4010-9213-c837316f8a30","d83bc577-1b03-4604-94a1-150ba7198ed0","6cba977a-462f-4d8c-b291-2dad991f85a0"]}</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B5" t="str">
         <f>_xlfn.CONCAT(
@@ -1785,12 +1785,12 @@
 CHAR(34), "spokeVmContAadGroupId", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", CHAR(34), appTeamsAadGroupObjectId, CHAR(34), "]},",
 CHAR(34), "spokeVmContributorsRoleAssignmentID", CHAR(34), ": {", CHAR(34), "value", CHAR(34), ":", "[", spokeVmContributorsRoleAssignmentID,"]}"
 )</f>
-        <v>"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24"]},"spokeVmContAadGroupId": {"value":["c2ecad99-6ed7-4e11-8acc-0fa0262a2c69"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6"]}</v>
+        <v>"spokeVnetName": {"value":["Spoke-Prod-EastUS2-01","Spoke-Test-EastUS2-01"]},"spokeVnetAddressSpace": {"value":["10.1.0.0/16","10.2.0.0/16"]},"spokeDeploySubscriptionResourceGroup": {"value":["","c64ca001-2cce-46de-837e-03f5564fc802/HubSpoke-02"]},"spokeSubnetBastionAddressSpace": {"value":["0.0.0.0/0"]},"spokeSubnetAppGwName": {"value":["AppGW"]},"spokeSubnetAppGwAddressSpace": {"value":["10.1.0.128/25","10.2.0.128/25"]},"spokeSubnet1Name": {"value":["Subnet1"]},"spokeSubnet1AddressSpace": {"value":["10.1.1.0/24","10.2.1.0/24"]},"spokeSubnet2Name": {"value":["Subnet2"]},"spokeSubnet2AddressSpace": {"value":["10.1.2.0/24","10.2.2.0/24"]},"spokeSubnet3Name": {"value":["Subnet3"]},"spokeSubnet3AddressSpace": {"value":["10.1.3.0/24","10.2.3.0/24"]},"spokeVmContAadGroupId": {"value":["002984bd-b5ce-445d-8138-d19b514550c7"]},"spokeVmContributorsRoleAssignmentID": {"value":["5a29e932-06c6-4e07-8e1b-d5f96c3524cf","ce7a113f-e760-4b94-a223-a52a1d2113d6"]}</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B6" t="str">
         <f>_xlfn.CONCAT(
@@ -1801,13 +1801,13 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B9" s="8"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B10" t="str">
         <f>IF(hubSubnetFirewallDeploy = "Deploy", hubSubnetFirewallAddressSpace, "0.0.0.0/0")</f>
@@ -1816,7 +1816,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B11" t="str">
         <f>IF(hubSubnetBastionDeploy = "Deploy", hubSubnetBastionAddressSpace, "0.0.0.0/0")</f>
@@ -1825,7 +1825,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B12" t="str">
         <f>IF(hubSubnetJumpHostsDeploy = "Deploy", hubSubnetJumpHostsAddressSpace, "0.0.0.0/0")</f>
@@ -1834,7 +1834,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B13" t="str">
         <f>IF(hubSubnet1Deploy = "Deploy", hubSubnet1AddressSpace, "0.0.0.0/0")</f>
@@ -1843,7 +1843,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B14" t="str">
         <f>IF(
@@ -1855,7 +1855,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B15" t="str">
         <f>IF(
@@ -1867,7 +1867,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B16" t="str">
         <f>IF(
@@ -1879,12 +1879,12 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B19" s="7" t="str">
         <f>_xlfn.CONCAT("""", Hub!D15, """", ",", """", Hub!D16, """")</f>
@@ -1893,7 +1893,7 @@
     </row>
     <row r="20" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B20" s="7" t="str">
         <f>_xlfn.CONCAT(
@@ -1911,13 +1911,13 @@
     <row r="22" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B23" s="8"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B24" t="str">
         <f>_xlfn.CONCAT(CHAR(34), Spoke1!$B$5, CHAR(34), ",", CHAR(34), Spoke2!$B$5, CHAR(34))</f>
@@ -1926,7 +1926,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B25" t="str">
         <f>_xlfn.CONCAT(CHAR(34), Spoke1!$C$5, CHAR(34), ",", CHAR(34), Spoke2!$C$5, CHAR(34))</f>
@@ -1935,7 +1935,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B26" t="str">
         <f>_xlfn.CONCAT(Spoke1!$D$2, ",", Spoke2!$D$2)</f>
@@ -1944,7 +1944,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B27" t="str">
         <f>IF(
@@ -1963,7 +1963,7 @@
     </row>
     <row r="28" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B28" s="5" t="str">
         <f>IF(
@@ -1976,7 +1976,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B29" s="3" t="str">
         <f>IF(
@@ -1995,7 +1995,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B30" s="5" t="str">
         <f>IF(
@@ -2008,7 +2008,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B31" s="3" t="str">
         <f>IF(
@@ -2027,7 +2027,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B32" s="5" t="str">
         <f>IF(
@@ -2040,7 +2040,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B33" s="3" t="str">
         <f>IF(
@@ -2059,7 +2059,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B34" s="5" t="str">
         <f>IF(
@@ -2072,7 +2072,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B35" s="3" t="str">
         <f>IF(
@@ -2094,7 +2094,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B36" t="str">
         <f>_xlfn.CONCAT("""",Spoke1!D15,"""",",","""",Spoke2!D15,"""")</f>
@@ -2135,46 +2135,46 @@
         <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="G1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed color for GUIDs for RBAC role assignments
</commit_message>
<xml_diff>
--- a/PowerShell/ParametersFileBuilder_2-Spoke.xlsx
+++ b/PowerShell/ParametersFileBuilder_2-Spoke.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark.bakunas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mark.bakunas\Documents\GitHub\Azure-HubSpoke\PowerShell\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9479735F-E74F-447C-B0A8-6233062D7E36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB79A3B9-D154-463B-96B9-5817E5DB14E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3600" yWindow="630" windowWidth="21600" windowHeight="14655" xr2:uid="{74A5C2AD-3876-4989-8818-24030CBF60E7}"/>
   </bookViews>
@@ -723,7 +723,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -742,6 +742,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -756,7 +762,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -773,6 +779,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1223,7 +1230,7 @@
       <c r="C18" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="14" t="s">
         <v>177</v>
       </c>
     </row>
@@ -1234,7 +1241,7 @@
       <c r="C19" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="14" t="s">
         <v>178</v>
       </c>
     </row>
@@ -1245,14 +1252,14 @@
       <c r="C20" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="14" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="D21" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1468,7 +1475,7 @@
       <c r="C18" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="14" t="s">
         <v>49</v>
       </c>
       <c r="E18" t="s">
@@ -1485,7 +1492,7 @@
       <c r="C19" t="s">
         <v>2</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="14" t="s">
         <v>50</v>
       </c>
       <c r="E19" t="str">
@@ -1503,7 +1510,7 @@
       <c r="C20" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="14" t="s">
         <v>54</v>
       </c>
       <c r="E20" t="str">
@@ -1521,7 +1528,7 @@
       <c r="C21" t="s">
         <v>8</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" s="14" t="s">
         <v>55</v>
       </c>
       <c r="E21" s="7" t="str">
@@ -1539,7 +1546,7 @@
       <c r="C22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="14" t="s">
         <v>56</v>
       </c>
       <c r="E22" s="7" t="str">
@@ -1559,7 +1566,7 @@
       <c r="C23" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="14" t="s">
         <v>57</v>
       </c>
       <c r="E23" s="7" t="str">
@@ -1579,7 +1586,7 @@
       <c r="C24" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" s="14" t="s">
         <v>58</v>
       </c>
       <c r="E24" s="7" t="str">
@@ -1599,7 +1606,7 @@
       <c r="C25" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="14" t="s">
         <v>94</v>
       </c>
       <c r="E25" t="s">
@@ -1782,12 +1789,12 @@
       <c r="C14" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="14" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="6" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1974,12 +1981,12 @@
       <c r="C14" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="14" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="6" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>